<commit_message>
Added 0x66 calibration, small code improvements
</commit_message>
<xml_diff>
--- a/Calibration.xlsx
+++ b/Calibration.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/43e0b09970218a64/Projects/Autonomie RAM/BatteryCurrent/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{BE1D8C51-0325-42D4-92BA-EBDA6328BFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{707A18C3-A9B8-4EE9-B533-DBEF0B9CDD53}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20445" yWindow="8400" windowWidth="16185" windowHeight="12120" xr2:uid="{D96A8E7D-5884-4797-A990-FD50B68563D6}"/>
+    <workbookView xWindow="20450" yWindow="8400" windowWidth="16190" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="0x65" sheetId="1" r:id="rId1"/>
+    <sheet name="0x66" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,8 +28,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>During calibration offset is +35</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,7 +87,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -98,6 +101,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -174,6 +178,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -301,7 +306,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B7C4-43F9-86B8-3654A5DBF550}"/>
             </c:ext>
@@ -315,11 +320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1301705248"/>
-        <c:axId val="1301696608"/>
+        <c:axId val="204151040"/>
+        <c:axId val="204152832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1301705248"/>
+        <c:axId val="204151040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,12 +381,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1301696608"/>
+        <c:crossAx val="204152832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1301696608"/>
+        <c:axId val="204152832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -438,7 +443,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1301705248"/>
+        <c:crossAx val="204151040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -487,560 +492,410 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'0x66'!$A$1:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>972</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1615</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-320.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-644</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-966</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'0x66'!$B$1:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-5001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B7C4-43F9-86B8-3654A5DBF550}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203887744"/>
+        <c:axId val="203889280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="203887744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="203889280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="203889280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="203887744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1063,11 +918,54 @@
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A1754B9-E2EF-9512-F383-385F9F431F11}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A1754B9-E2EF-9512-F383-385F9F431F11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A1754B9-E2EF-9512-F383-385F9F431F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1127,7 +1025,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1179,7 +1077,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1373,21 +1271,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741A9133-21B6-46E3-BFCF-C9223958E5D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -1469,7 +1367,7 @@
         <v>-655.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>-3004</v>
       </c>
@@ -1477,7 +1375,7 @@
         <v>-984</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>-4000</v>
       </c>
@@ -1485,12 +1383,137 @@
         <v>-1309.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>-5001</v>
       </c>
       <c r="B13">
         <v>-1638.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>326</v>
+      </c>
+      <c r="B3">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>649</v>
+      </c>
+      <c r="B4">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>972</v>
+      </c>
+      <c r="B5">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1292</v>
+      </c>
+      <c r="B6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1615</v>
+      </c>
+      <c r="B7">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-160</v>
+      </c>
+      <c r="B8">
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>-320.5</v>
+      </c>
+      <c r="B9">
+        <v>-1002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>-644</v>
+      </c>
+      <c r="B10">
+        <v>-2004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>-966</v>
+      </c>
+      <c r="B11">
+        <v>-3004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-1288</v>
+      </c>
+      <c r="B12">
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>-1611</v>
+      </c>
+      <c r="B13">
+        <v>-5001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>